<commit_message>
New election files for 03.10.2017-21.10.2017
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="231">
   <si>
     <t xml:space="preserve">ქართული ოცნება</t>
   </si>
@@ -704,6 +704,15 @@
   </si>
   <si>
     <t xml:space="preserve">People's Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">საქართველოს ერთობისა და განვითარების პარტია</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unity of Georgia and Development Party </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Партия единства и развития Грузии</t>
   </si>
 </sst>
 </file>
@@ -813,22 +822,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D82" activeCellId="0" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2363,6 +2374,20 @@
       </c>
       <c r="E81" s="1" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add annual for 2017 for 21 parties
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="237">
   <si>
     <t xml:space="preserve">ქართული ოცნება</t>
   </si>
@@ -713,6 +713,24 @@
   </si>
   <si>
     <t xml:space="preserve">Партия единства и развития Грузии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">მოძრაობა თავისუფალი საქართველოსთვის</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movement for Free Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Движение за Свободную Грузию</t>
+  </si>
+  <si>
+    <t xml:space="preserve">საქართველოს ძალოვან ვეტერანთა და პატრიოტთა პოლიტიკური მოძრაობა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Political Movement of Law Enforcement Veterans and Patriots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Политическое движение грузинских ветеранов и патриотов</t>
   </si>
 </sst>
 </file>
@@ -822,24 +840,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D82" activeCellId="0" sqref="D82"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E84" activeCellId="0" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2388,6 +2405,34 @@
       </c>
       <c r="E82" s="1" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare election files for upload
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="238">
   <si>
     <t xml:space="preserve">ქართული ოცნება</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t xml:space="preserve">Политическое движение грузинских ветеранов и патриотов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ახალი ქრისტიან-დემოკრატები</t>
   </si>
 </sst>
 </file>
@@ -840,23 +843,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E84" activeCellId="0" sqref="E84"/>
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.0663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.9948979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2433,6 +2435,20 @@
       </c>
       <c r="E84" s="1" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>